<commit_message>
correção no sistema de moedas
</commit_message>
<xml_diff>
--- a/robo_mktplace.xlsx
+++ b/robo_mktplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\python projects\marketplace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucim\Documents\pyprojects\yapo-marketplace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A52EEE2-8902-4831-9D36-C88531B64B36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87824D88-EA48-4F1D-978B-00115E13838C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>camisaseleção.xlsx</t>
   </si>
   <si>
-    <t>Camiseta</t>
+    <t>Moto</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:AMI3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
id tirado dos produtos e virgula no lugar de ponto
</commit_message>
<xml_diff>
--- a/robo_mktplace.xlsx
+++ b/robo_mktplace.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucim\Documents\pyprojects\yapo-marketplace\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87824D88-EA48-4F1D-978B-00115E13838C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -42,39 +31,381 @@
     <t>OUTPUT_FILE</t>
   </si>
   <si>
-    <t>camisaseleção.xlsx</t>
+    <t>camisa</t>
   </si>
   <si>
-    <t>Moto</t>
+    <t>camisaseleção.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -121,9 +452,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -133,17 +706,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="40% - Ênfase 4" xfId="3" builtinId="43"/>
+    <cellStyle name="Porcentagem" xfId="4" builtinId="5"/>
+    <cellStyle name="Célula Vinculada" xfId="5" builtinId="24"/>
+    <cellStyle name="Célula de Verificação" xfId="6" builtinId="23"/>
+    <cellStyle name="Moeda [0]" xfId="7" builtinId="7"/>
+    <cellStyle name="20% - Ênfase 3" xfId="8" builtinId="38"/>
+    <cellStyle name="Moeda" xfId="9" builtinId="4"/>
+    <cellStyle name="Hyperlink seguido" xfId="10" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
+    <cellStyle name="40% - Ênfase 2" xfId="12" builtinId="35"/>
+    <cellStyle name="Observação" xfId="13" builtinId="10"/>
+    <cellStyle name="40% - Ênfase 6" xfId="14" builtinId="51"/>
+    <cellStyle name="Texto de Aviso" xfId="15" builtinId="11"/>
+    <cellStyle name="Título" xfId="16" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="17" builtinId="53"/>
+    <cellStyle name="Ênfase 3" xfId="18" builtinId="37"/>
+    <cellStyle name="Título 1" xfId="19" builtinId="16"/>
+    <cellStyle name="Ênfase 4" xfId="20" builtinId="41"/>
+    <cellStyle name="Título 2" xfId="21" builtinId="17"/>
+    <cellStyle name="Ênfase 5" xfId="22" builtinId="45"/>
+    <cellStyle name="Título 3" xfId="23" builtinId="18"/>
+    <cellStyle name="Ênfase 6" xfId="24" builtinId="49"/>
+    <cellStyle name="Título 4" xfId="25" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="26" builtinId="20"/>
+    <cellStyle name="Saída" xfId="27" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="28" builtinId="22"/>
+    <cellStyle name="Total" xfId="29" builtinId="25"/>
+    <cellStyle name="40% - Ênfase 1" xfId="30" builtinId="31"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="32" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="33" builtinId="28"/>
+    <cellStyle name="20% - Ênfase 5" xfId="34" builtinId="46"/>
+    <cellStyle name="Ênfase 1" xfId="35" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="36" builtinId="30"/>
+    <cellStyle name="60% - Ênfase 1" xfId="37" builtinId="32"/>
+    <cellStyle name="20% - Ênfase 6" xfId="38" builtinId="50"/>
+    <cellStyle name="Ênfase 2" xfId="39" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="40" builtinId="34"/>
+    <cellStyle name="60% - Ênfase 2" xfId="41" builtinId="36"/>
+    <cellStyle name="40% - Ênfase 3" xfId="42" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="43" builtinId="40"/>
+    <cellStyle name="20% - Ênfase 4" xfId="44" builtinId="42"/>
+    <cellStyle name="60% - Ênfase 4" xfId="45" builtinId="44"/>
+    <cellStyle name="40% - Ênfase 5" xfId="46" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="47" builtinId="48"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +809,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +844,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,34 +1018,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="1023" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="62.5714285714286" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.14285714285714" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7142857142857" style="1" customWidth="1"/>
+    <col min="6" max="1023" width="9.14285714285714" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -445,23 +1057,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>200</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5"/>
       <c r="E3" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aba Código do produto add
</commit_message>
<xml_diff>
--- a/robo_mktplace.xlsx
+++ b/robo_mktplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\python projects\yapo-marketplace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\python_projects\yapo-marketplace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13D5D7-2399-49C9-A827-ED062A6B1D4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485A252A-4BE1-4057-B2FF-227045297533}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NOME_SITE</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>camisaseleção.xlsx</t>
-  </si>
-  <si>
-    <t>200.4</t>
   </si>
 </sst>
 </file>
@@ -441,8 +438,8 @@
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+      <c r="D2" s="1">
+        <v>299</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
@@ -454,6 +451,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>